<commit_message>
took prescaler into calculation
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DROPBOX\Dropbox\WORKSPACE_AVR\___VSCODE\tiny13-ir-nec\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DROPBOX\Dropbox\WORKSPACE_AVR\___VSCODE\attiny-ir-nec-decoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0427F5-462E-4510-976A-51AF94C2BFE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5690D-63EC-461B-AC2B-900BECABDC86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1F3E930-A99F-4142-90E6-5A15EC684D90}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>F_CPU</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>AVR TIMINGS</t>
+  </si>
+  <si>
+    <t>Prescaler</t>
   </si>
 </sst>
 </file>
@@ -341,15 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -362,6 +356,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
@@ -680,204 +683,208 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="4" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="6"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>1000000</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="8"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2">
         <v>562.5</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="9" t="s">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="2">
         <v>1687.5</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <f>B2/2^B3</f>
+        <f>B2/B4/2^B3</f>
         <v>3906.25</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="10"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
         <f>1/B5*1000000</f>
         <v>256</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="8"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2">
         <v>562.5</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="2">
         <v>562.5</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3">
         <f>E3/B6</f>
         <v>2.197265625</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="9"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3">
         <f>E4/B6</f>
         <v>6.591796875</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3">
         <f>E11/B6</f>
         <v>35.15625</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="2">
         <v>9000</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="14">
         <f>E12/B6</f>
         <v>17.578125</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="10">
         <v>4500</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="11" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>